<commit_message>
merge gwlevel/drawdown correction phreatic scheme
</commit_message>
<xml_diff>
--- a/testing/test11_phrea/results/phreatic_summary_traveltimes_anaysis_SR220901.xlsx
+++ b/testing/test11_phrea/results/phreatic_summary_traveltimes_anaysis_SR220901.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sutra2_tool\sutra2\testing\test11_phrea\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1BD12456-D6EE-4C3D-9209-DF69AD8AB4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED6EAE6-E9D6-4A29-811A-249B2349CD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phreatic_summary_traveltimes_an" sheetId="1" r:id="rId1"/>
     <sheet name="phreatic_summary_traveltimes_mo" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>total_travel_time</t>
   </si>
@@ -55,11 +67,23 @@
   <si>
     <t>travel_time_sat_AW</t>
   </si>
+  <si>
+    <t>MPW class no gp</t>
+  </si>
+  <si>
+    <t>travel_time_sat_MPW_nogp</t>
+  </si>
+  <si>
+    <t>travel_time_vadose_zone_nogp</t>
+  </si>
+  <si>
+    <t>travel_time_vadose_zone_withgp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2690,6 +2714,1061 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-4A65-4FB3-9030-1963AC0F9A39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>phreatic_summary_traveltimes_an!$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>travel_time_sat_MPW_nogp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$R$3:$R$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.36549997329711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3469998836517298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3284997940063397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3095002174377397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2904996871948207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.271499633789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.2530002593994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.234499931335399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.215499877929599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.19700050354</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.178499221801701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.159500122070298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.140499114990199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.1215000152587</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.103000640869102</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.084499359130799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.065498352050703</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35.047000885009702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.028499603271399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39.009498596191399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>68.124496459960895</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>124.373497009277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>180.62249755859301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>236.87150573730401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>293.120513916015</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>349.36950683593699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>405.61849975585898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>461.86749267578102</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>518.11651611328102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>574.365478515625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>630.614501953125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>686.86358642578102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>743.11248779296795</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>799.36151123046795</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>855.61047363281205</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>911.85949707031205</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>968.10852050781205</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1024.35754394531</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1080.6064453125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1136.85546875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1193.10498046875</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1249.3544921875</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1305.603515625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1361.8525390625</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1418.10144042968</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1474.35046386718</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1530.59948730468</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1586.84851074218</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1643.09753417968</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1699.34655761718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$W$3:$W$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>17.253173828119998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.643798828119998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.472412109369998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.189453125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.62939453125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.617919921880002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.199462890619998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76.052001953119998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.53515625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>105.22192382813</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>122.90576171875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>142.83178710938</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>164.275390625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>187.97375488281</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>215.80249023437</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>239.0625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>258.91271972656</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>283.56030273438</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>310.11987304687</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>335.21960449219</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1172.34545898437</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3146.27880859375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3597.2828369140698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4078.7783203125</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4781.41357421875</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4548.9639892578198</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4835.4666748046902</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5171.2474365234402</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5560.79345703125</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6005.9158935546902</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6509.2421875</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7074.1959228515698</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7705.1607666015698</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8407.5755615234393</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9188.2141113281305</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10055.3857421875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11019.38720703125</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12093.12841796875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13292.867553710939</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14639.45922851563</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16160.21484375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>17891.58361816407</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19883.828125</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>22208.770385742191</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>24974.101928710941</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>28351.89025878907</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>32643.22961425782</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>38453.947631835938</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47344.92492675782</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>66622.973388671875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94FE-405D-90C7-5E0861ACF6E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>phreatic_summary_traveltimes_an!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>travel_time_vadose_zone_nogp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$R$3:$R$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.36549997329711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3469998836517298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3284997940063397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3095002174377397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2904996871948207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.271499633789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.2530002593994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.234499931335399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.215499877929599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.19700050354</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.178499221801701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.159500122070298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.140499114990199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.1215000152587</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.103000640869102</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.084499359130799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.065498352050703</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35.047000885009702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.028499603271399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39.009498596191399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>68.124496459960895</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>124.373497009277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>180.62249755859301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>236.87150573730401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>293.120513916015</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>349.36950683593699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>405.61849975585898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>461.86749267578102</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>518.11651611328102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>574.365478515625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>630.614501953125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>686.86358642578102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>743.11248779296795</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>799.36151123046795</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>855.61047363281205</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>911.85949707031205</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>968.10852050781205</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1024.35754394531</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1080.6064453125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1136.85546875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1193.10498046875</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1249.3544921875</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1305.603515625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1361.8525390625</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1418.10144042968</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1474.35046386718</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1530.59948730468</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1586.84851074218</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1643.09753417968</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1699.34655761718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$T$3:$T$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2435.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2399.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2345.22509765625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2279.40014648437</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2248.05004882812</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2238.27514648437</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2222.27490234375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2178.84985351562</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2153.82495117187</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2127.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2100.72485351562</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2073.4501953125</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2046.02502441406</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018.625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1999.92504882812</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1998.77502441406</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1996.42504882812</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1993.02490234375</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1988.52502441406</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1885.47509765625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1741.35009765625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1687.59997558593</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1618.25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1546.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1499.47497558593</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1493.04992675781</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1481.79992675781</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1467.72509765625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1452.04992675781</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1435.625</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1418.97497558593</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1402.47497558593</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1386.40002441406</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1370.94995117187</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1356.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1342.39990234375</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1329.47509765625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1317.52502441406</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1306.57495117187</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1296.625</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1287.72497558593</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1279.875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1273.04992675781</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1267.27502441406</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1262.47497558593</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1258.70007324218</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1255.90002441406</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1254.07507324218</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1253.17504882812</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-94FE-405D-90C7-5E0861ACF6E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>phreatic_summary_traveltimes_an!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>travel_time_vadose_zone_withgp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$J$3:$J$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.36549997329711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3469998836517298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3284997940063397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3095002174377397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2904996871948207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.271499633789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.2530002593994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.234499931335399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.215499877929599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.19700050354</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.178499221801701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.159500122070298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.140499114990199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.1215000152587</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.103000640869102</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.084499359130799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.065498352050703</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35.047000885009702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.028499603271399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39.009498596191399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>68.124496459960895</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>124.373497009277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>180.62249755859301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>236.87150573730401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>293.120513916015</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>349.36950683593699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>405.61849975585898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>461.86749267578102</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>518.11651611328102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>574.365478515625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>630.614501953125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>686.86358642578102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>743.11248779296795</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>799.36151123046795</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>855.61047363281205</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>911.85949707031205</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>968.10852050781205</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1024.35754394531</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1080.6064453125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1136.85546875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1193.10498046875</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1249.3544921875</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1305.603515625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1361.8525390625</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1418.10144042968</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1474.35046386718</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1530.59948730468</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1586.84851074218</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1643.09753417968</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1699.34655761718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>phreatic_summary_traveltimes_an!$L$3:$L$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2435.52490234375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2400.7001953125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2281.60009765625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2248.27514648437</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2238.77490234375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2202.92504882812</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2179.97509765625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2155.10009765625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2129.05004882812</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2102.27490234375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2075.09985351562</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2047.80004882812</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1999.95007324218</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1998.90002441406</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1996.65002441406</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1993.34997558593</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1988.95007324218</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1886.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1741.70007324218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1688.55004882812</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1619.625</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1548.19995117187</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1499.54992675781</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1493.34997558593</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1482.30004882812</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1468.40002441406</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1452.875</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1436.57507324218</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1420.05004882812</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1403.65002441406</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1387.67504882812</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1372.30004882812</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1357.67492675781</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1343.90002441406</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1331.02502441406</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1319.125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1308.22497558593</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1298.32495117187</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1289.47497558593</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1281.64990234375</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1274.84997558593</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1269.07507324218</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1264.32507324218</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1260.55004882812</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1257.77490234375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1255.94995117187</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1255.02502441406</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-94FE-405D-90C7-5E0861ACF6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3774,24 +4853,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -3817,7 +4899,7 @@
         <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -3828,8 +4910,26 @@
       <c r="O2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3874,8 +4974,24 @@
         <f>K3-L3</f>
         <v>18.126953125</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1.36549997329711</v>
+      </c>
+      <c r="S3">
+        <v>2452.87817382812</v>
+      </c>
+      <c r="T3">
+        <v>2435.625</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W52" si="0">S3-T3</f>
+        <v>17.253173828119998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3895,7 +5011,7 @@
         <v>1.75008750583232</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G67" si="0">C4-D4</f>
+        <f t="shared" ref="G4:G67" si="1">C4-D4</f>
         <v>2658.9322776321696</v>
       </c>
       <c r="I4">
@@ -3917,11 +5033,27 @@
         <v>1.953125E-3</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O67" si="1">K4-L4</f>
+        <f t="shared" ref="O4:O52" si="2">K4-L4</f>
         <v>22.128173828119998</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>3.3469998836517298</v>
+      </c>
+      <c r="S4">
+        <v>2421.26879882812</v>
+      </c>
+      <c r="T4">
+        <v>2399.625</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>21.643798828119998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3941,7 +5073,7 @@
         <v>17.508755837713299</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3104.1453984324698</v>
       </c>
       <c r="I5">
@@ -3963,11 +5095,27 @@
         <v>2.197265625E-3</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.828125</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>5.3284997940063397</v>
+      </c>
+      <c r="S5">
+        <v>2374.69750976562</v>
+      </c>
+      <c r="T5">
+        <v>2345.22509765625</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>29.472412109369998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3987,7 +5135,7 @@
         <v>87.719481912023298</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3474.5319050107496</v>
       </c>
       <c r="I6">
@@ -4009,11 +5157,27 @@
         <v>1.46484375E-3</v>
       </c>
       <c r="O6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43.426513671869998</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>7.3095002174377397</v>
+      </c>
+      <c r="S6">
+        <v>2322.58959960937</v>
+      </c>
+      <c r="T6">
+        <v>2279.40014648437</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>43.189453125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4033,7 +5197,7 @@
         <v>175.88087743627599</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3691.9719724994397</v>
       </c>
       <c r="I7">
@@ -4055,11 +5219,27 @@
         <v>1.953125E-3</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50.247802734380002</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>9.2904996871948207</v>
+      </c>
+      <c r="S7">
+        <v>2297.67944335937</v>
+      </c>
+      <c r="T7">
+        <v>2248.05004882812</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>49.62939453125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4079,7 +5259,7 @@
         <v>353.54737805658999</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3998.91714508421</v>
       </c>
       <c r="I8">
@@ -4101,11 +5281,27 @@
         <v>3.662109375E-3</v>
       </c>
       <c r="O8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54.76416015625</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>11.271499633789</v>
+      </c>
+      <c r="S8">
+        <v>2292.89306640625</v>
+      </c>
+      <c r="T8">
+        <v>2238.27514648437</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>54.617919921880002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4125,7 +5321,7 @@
         <v>533.036130982401</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4254.0290732522499</v>
       </c>
       <c r="I9">
@@ -4147,11 +5343,27 @@
         <v>5.126953125E-3</v>
       </c>
       <c r="O9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.22509765625</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>13.2530002593994</v>
+      </c>
+      <c r="S9">
+        <v>2286.47436523437</v>
+      </c>
+      <c r="T9">
+        <v>2222.27490234375</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>64.199462890619998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4171,7 +5383,7 @@
         <v>714.38490410446605</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4489.0333430965202</v>
       </c>
       <c r="I10">
@@ -4193,11 +5405,27 @@
         <v>5.859375E-3</v>
       </c>
       <c r="O10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75.92041015625</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>15.234499931335399</v>
+      </c>
+      <c r="S10">
+        <v>2278.05200195312</v>
+      </c>
+      <c r="T10">
+        <v>2202</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>76.052001953119998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4217,7 +5445,7 @@
         <v>897.63265178213305</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4713.8995273492701</v>
       </c>
       <c r="I11">
@@ -4239,11 +5467,27 @@
         <v>6.34765625E-3</v>
       </c>
       <c r="O11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.391357421869998</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>17.215499877929599</v>
+      </c>
+      <c r="S11">
+        <v>2268.38500976562</v>
+      </c>
+      <c r="T11">
+        <v>2178.84985351562</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="0"/>
+        <v>89.53515625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4263,7 +5507,7 @@
         <v>1082.81956506653</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4933.0911793008308</v>
       </c>
       <c r="I12">
@@ -4285,11 +5529,27 @@
         <v>6.34765625E-3</v>
       </c>
       <c r="O12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105.04858398437</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>19.19700050354</v>
+      </c>
+      <c r="S12">
+        <v>2259.046875</v>
+      </c>
+      <c r="T12">
+        <v>2153.82495117187</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>105.22192382813</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4309,7 +5569,7 @@
         <v>1269.98712460961</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5149.0093357292399</v>
       </c>
       <c r="I13">
@@ -4331,11 +5591,27 @@
         <v>6.34765625E-3</v>
       </c>
       <c r="O13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.66943359375</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>21.178499221801701</v>
+      </c>
+      <c r="S13">
+        <v>2250.53076171875</v>
+      </c>
+      <c r="T13">
+        <v>2127.625</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="0"/>
+        <v>122.90576171875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4355,7 +5631,7 @@
         <v>1459.1781564333901</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5363.1052673898994</v>
       </c>
       <c r="I14">
@@ -4377,11 +5653,27 @@
         <v>5.859375E-3</v>
       </c>
       <c r="O14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142.4697265625</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>23.159500122070298</v>
+      </c>
+      <c r="S14">
+        <v>2243.556640625</v>
+      </c>
+      <c r="T14">
+        <v>2100.72485351562</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>142.83178710938</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4401,7 +5693,7 @@
         <v>1650.4368907467201</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5576.3316802232494</v>
       </c>
       <c r="I15">
@@ -4423,11 +5715,27 @@
         <v>5.126953125E-3</v>
       </c>
       <c r="O15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>164.1240234375</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <v>12</v>
+      </c>
+      <c r="R15">
+        <v>25.140499114990199</v>
+      </c>
+      <c r="S15">
+        <v>2237.7255859375</v>
+      </c>
+      <c r="T15">
+        <v>2073.4501953125</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>164.275390625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4447,7 +5755,7 @@
         <v>1843.80902401196</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5789.3545715435494</v>
       </c>
       <c r="I16">
@@ -4469,11 +5777,27 @@
         <v>4.150390625E-3</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>187.59423828125</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>27.1215000152587</v>
+      </c>
+      <c r="S16">
+        <v>2233.99877929687</v>
+      </c>
+      <c r="T16">
+        <v>2046.02502441406</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="0"/>
+        <v>187.97375488281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4493,7 +5817,7 @@
         <v>2039.34178447915</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6002.66360495156</v>
       </c>
       <c r="I17">
@@ -4515,11 +5839,27 @@
         <v>2.44140625E-3</v>
       </c>
       <c r="O17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215.45849609375</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q17">
+        <v>14</v>
+      </c>
+      <c r="R17">
+        <v>29.103000640869102</v>
+      </c>
+      <c r="S17">
+        <v>2234.42749023437</v>
+      </c>
+      <c r="T17">
+        <v>2018.625</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="0"/>
+        <v>215.80249023437</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4539,7 +5879,7 @@
         <v>2237.0840014229798</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6216.6342876217204</v>
       </c>
       <c r="I18">
@@ -4561,11 +5901,27 @@
         <v>2.9296875E-3</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>239.35876464844</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <v>15</v>
+      </c>
+      <c r="R18">
+        <v>31.084499359130799</v>
+      </c>
+      <c r="S18">
+        <v>2238.98754882812</v>
+      </c>
+      <c r="T18">
+        <v>1999.92504882812</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="0"/>
+        <v>239.0625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4585,7 +5941,7 @@
         <v>2437.0861783363798</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6431.5652058453106</v>
       </c>
       <c r="I19">
@@ -4607,11 +5963,27 @@
         <v>6.103515625E-3</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>258.85900878906</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q19">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>33.065498352050703</v>
+      </c>
+      <c r="S19">
+        <v>2257.68774414062</v>
+      </c>
+      <c r="T19">
+        <v>1998.77502441406</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="0"/>
+        <v>258.91271972656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4631,7 +6003,7 @@
         <v>2639.4005703552102</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6647.7014534392902</v>
       </c>
       <c r="I20">
@@ -4653,11 +6025,27 @@
         <v>9.033203125E-3</v>
       </c>
       <c r="O20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>283.39685058594</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <v>17</v>
+      </c>
+      <c r="R20">
+        <v>35.047000885009702</v>
+      </c>
+      <c r="S20">
+        <v>2279.9853515625</v>
+      </c>
+      <c r="T20">
+        <v>1996.42504882812</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="0"/>
+        <v>283.56030273438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4677,7 +6065,7 @@
         <v>2844.0812662110602</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6865.2499889848796</v>
       </c>
       <c r="I21">
@@ -4699,11 +6087,27 @@
         <v>1.171875E-2</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>309.93395996094</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q21">
+        <v>18</v>
+      </c>
+      <c r="R21">
+        <v>37.028499603271399</v>
+      </c>
+      <c r="S21">
+        <v>2303.14477539062</v>
+      </c>
+      <c r="T21">
+        <v>1993.02490234375</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="0"/>
+        <v>310.11987304687</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4723,7 +6127,7 @@
         <v>3051.18427503361</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7084.3900579545498</v>
       </c>
       <c r="I22">
@@ -4745,11 +6149,27 @@
         <v>1.5625E-2</v>
       </c>
       <c r="O22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>335.00354003907</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q22">
+        <v>19</v>
+      </c>
+      <c r="R22">
+        <v>39.009498596191399</v>
+      </c>
+      <c r="S22">
+        <v>2323.74462890625</v>
+      </c>
+      <c r="T22">
+        <v>1988.52502441406</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="0"/>
+        <v>335.21960449219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4769,7 +6189,7 @@
         <v>3260.7676183511298</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7305.2804812351696</v>
       </c>
       <c r="I23">
@@ -4791,11 +6211,27 @@
         <v>6.93359375E-2</v>
       </c>
       <c r="O23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1171.01025390625</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q23">
+        <v>20</v>
+      </c>
+      <c r="R23">
+        <v>68.124496459960895</v>
+      </c>
+      <c r="S23">
+        <v>3057.82055664062</v>
+      </c>
+      <c r="T23">
+        <v>1885.47509765625</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="0"/>
+        <v>1172.34545898437</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4815,7 +6251,7 @@
         <v>3472.8914276671599</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7528.064889108131</v>
       </c>
       <c r="I24">
@@ -4837,11 +6273,27 @@
         <v>7.75732421875</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3146.1153564453198</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q24">
+        <v>21</v>
+      </c>
+      <c r="R24">
+        <v>124.373497009277</v>
+      </c>
+      <c r="S24">
+        <v>4887.62890625</v>
+      </c>
+      <c r="T24">
+        <v>1741.35009765625</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="0"/>
+        <v>3146.27880859375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4861,7 +6313,7 @@
         <v>3687.61804802391</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7752.8755706263</v>
       </c>
       <c r="I25">
@@ -4883,11 +6335,27 @@
         <v>98.6083984375</v>
       </c>
       <c r="O25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3595.10717773438</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q25">
+        <v>22</v>
+      </c>
+      <c r="R25">
+        <v>180.62249755859301</v>
+      </c>
+      <c r="S25">
+        <v>5284.8828125</v>
+      </c>
+      <c r="T25">
+        <v>1687.59997558593</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="0"/>
+        <v>3597.2828369140698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4907,7 +6375,7 @@
         <v>3905.0121479986701</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7979.8363674946895</v>
       </c>
       <c r="I26">
@@ -4929,11 +6397,27 @@
         <v>229.46484375</v>
       </c>
       <c r="O26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4072.646484375</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q26">
+        <v>23</v>
+      </c>
+      <c r="R26">
+        <v>236.87150573730401</v>
+      </c>
+      <c r="S26">
+        <v>5697.0283203125</v>
+      </c>
+      <c r="T26">
+        <v>1618.25</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="0"/>
+        <v>4078.7783203125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4953,7 +6437,7 @@
         <v>4125.1408366187197</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8209.0648949450206</v>
       </c>
       <c r="I27">
@@ -4975,11 +6459,27 @@
         <v>395.2001953125</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4763.0197753906305</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q27">
+        <v>24</v>
+      </c>
+      <c r="R27">
+        <v>293.120513916015</v>
+      </c>
+      <c r="S27">
+        <v>6327.91357421875</v>
+      </c>
+      <c r="T27">
+        <v>1546.5</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="0"/>
+        <v>4781.41357421875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4999,7 +6499,7 @@
         <v>4348.0737877237398</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8440.6742801605906</v>
       </c>
       <c r="I28">
@@ -5021,11 +6521,27 @@
         <v>628.56689453125</v>
       </c>
       <c r="O28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4549.1942138671902</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q28">
+        <v>25</v>
+      </c>
+      <c r="R28">
+        <v>349.36950683593699</v>
+      </c>
+      <c r="S28">
+        <v>6048.43896484375</v>
+      </c>
+      <c r="T28">
+        <v>1499.47497558593</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="0"/>
+        <v>4548.9639892578198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5045,7 +6561,7 @@
         <v>4573.8833723521302</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8674.7745496431908</v>
       </c>
       <c r="I29">
@@ -5067,11 +6583,27 @@
         <v>890.97021484375</v>
       </c>
       <c r="O29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4834.8438720703198</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q29">
+        <v>26</v>
+      </c>
+      <c r="R29">
+        <v>405.61849975585898</v>
+      </c>
+      <c r="S29">
+        <v>6328.5166015625</v>
+      </c>
+      <c r="T29">
+        <v>1493.04992675781</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="0"/>
+        <v>4835.4666748046902</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5091,7 +6623,7 @@
         <v>4802.6447997808</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8911.4737579439388</v>
       </c>
       <c r="I30">
@@ -5113,11 +6645,27 @@
         <v>1197.7509765625</v>
       </c>
       <c r="O30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5170.1374511718805</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q30">
+        <v>27</v>
+      </c>
+      <c r="R30">
+        <v>461.86749267578102</v>
+      </c>
+      <c r="S30">
+        <v>6653.04736328125</v>
+      </c>
+      <c r="T30">
+        <v>1481.79992675781</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="0"/>
+        <v>5171.2474365234402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5137,7 +6685,7 @@
         <v>5034.4362679061596</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9150.8789239772486</v>
       </c>
       <c r="I31">
@@ -5159,11 +6707,27 @@
         <v>1550.81884765625</v>
       </c>
       <c r="O31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5559.1634521484402</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q31">
+        <v>28</v>
+      </c>
+      <c r="R31">
+        <v>518.11651611328102</v>
+      </c>
+      <c r="S31">
+        <v>7028.5185546875</v>
+      </c>
+      <c r="T31">
+        <v>1467.72509765625</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="0"/>
+        <v>5560.79345703125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5183,7 +6747,7 @@
         <v>5269.3391237186197</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9393.0968231919487</v>
       </c>
       <c r="I32">
@@ -5205,11 +6769,27 @@
         <v>1952.94921875</v>
       </c>
       <c r="O32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6003.7412109375</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q32">
+        <v>29</v>
+      </c>
+      <c r="R32">
+        <v>574.365478515625</v>
+      </c>
+      <c r="S32">
+        <v>7457.9658203125</v>
+      </c>
+      <c r="T32">
+        <v>1452.04992675781</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="0"/>
+        <v>6005.9158935546902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5229,7 +6809,7 @@
         <v>5507.4380346947501</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9638.2346713779298</v>
       </c>
       <c r="I33">
@@ -5251,11 +6831,27 @@
         <v>2407.45166015625</v>
       </c>
       <c r="O33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6506.4517822265698</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q33">
+        <v>30</v>
+      </c>
+      <c r="R33">
+        <v>630.614501953125</v>
+      </c>
+      <c r="S33">
+        <v>7944.8671875</v>
+      </c>
+      <c r="T33">
+        <v>1435.625</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="0"/>
+        <v>6509.2421875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5275,7 +6871,7 @@
         <v>5748.8211720106301</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9886.4007270591392</v>
       </c>
       <c r="I34">
@@ -5297,11 +6893,27 @@
         <v>2918.2705078125</v>
       </c>
       <c r="O34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7070.7204589843805</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q34">
+        <v>31</v>
+      </c>
+      <c r="R34">
+        <v>686.86358642578102</v>
+      </c>
+      <c r="S34">
+        <v>8493.1708984375</v>
+      </c>
+      <c r="T34">
+        <v>1418.97497558593</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="0"/>
+        <v>7074.1959228515698</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5321,7 +6933,7 @@
         <v>5993.5804065685797</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10137.70483311032</v>
       </c>
       <c r="I35">
@@ -5343,11 +6955,27 @@
         <v>3490.12109375</v>
       </c>
       <c r="O35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7700.9173583984402</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q35">
+        <v>32</v>
+      </c>
+      <c r="R35">
+        <v>743.11248779296795</v>
+      </c>
+      <c r="S35">
+        <v>9107.6357421875</v>
+      </c>
+      <c r="T35">
+        <v>1402.47497558593</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="0"/>
+        <v>7705.1607666015698</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5367,7 +6995,7 @@
         <v>6241.8115189278096</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10392.25891366603</v>
       </c>
       <c r="I36">
@@ -5389,11 +7017,27 @@
         <v>4128.6533203125</v>
       </c>
       <c r="O36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8402.4733886718805</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q36">
+        <v>33</v>
+      </c>
+      <c r="R36">
+        <v>799.36151123046795</v>
+      </c>
+      <c r="S36">
+        <v>9793.9755859375</v>
+      </c>
+      <c r="T36">
+        <v>1386.40002441406</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="0"/>
+        <v>8407.5755615234393</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5413,7 +7057,7 @@
         <v>6493.6144243395602</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10650.177439060641</v>
       </c>
       <c r="I37">
@@ -5435,11 +7079,27 @@
         <v>4840.6875</v>
       </c>
       <c r="O37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9182.1062011718805</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q37">
+        <v>34</v>
+      </c>
+      <c r="R37">
+        <v>855.61047363281205</v>
+      </c>
+      <c r="S37">
+        <v>10559.1640625</v>
+      </c>
+      <c r="T37">
+        <v>1370.94995117187</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="0"/>
+        <v>9188.2141113281305</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5459,7 +7119,7 @@
         <v>6749.0934142097303</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10911.577869095099</v>
       </c>
       <c r="I38">
@@ -5481,11 +7141,27 @@
         <v>5634.50927734375</v>
       </c>
       <c r="O38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10048.100463867189</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q38">
+        <v>35</v>
+      </c>
+      <c r="R38">
+        <v>911.85949707031205</v>
+      </c>
+      <c r="S38">
+        <v>11411.6357421875</v>
+      </c>
+      <c r="T38">
+        <v>1356.25</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="0"/>
+        <v>10055.3857421875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5505,7 +7181,7 @@
         <v>7008.3574154496901</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11176.58108312872</v>
       </c>
       <c r="I39">
@@ -5527,11 +7203,27 @@
         <v>6520.2890625</v>
       </c>
       <c r="O39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11010.724975585939</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q39">
+        <v>36</v>
+      </c>
+      <c r="R39">
+        <v>968.10852050781205</v>
+      </c>
+      <c r="S39">
+        <v>12361.787109375</v>
+      </c>
+      <c r="T39">
+        <v>1342.39990234375</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="0"/>
+        <v>11019.38720703125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5551,7 +7243,7 @@
         <v>7271.5202693291503</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11445.311804177631</v>
       </c>
       <c r="I40">
@@ -5573,11 +7265,27 @@
         <v>7510.64794921875</v>
       </c>
       <c r="O40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12082.790405273439</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q40">
+        <v>37</v>
+      </c>
+      <c r="R40">
+        <v>1024.35754394531</v>
+      </c>
+      <c r="S40">
+        <v>13422.603515625</v>
+      </c>
+      <c r="T40">
+        <v>1329.47509765625</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="0"/>
+        <v>12093.12841796875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5597,7 +7305,7 @@
         <v>7538.7010316179503</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11717.899023241531</v>
       </c>
       <c r="I41">
@@ -5619,11 +7327,27 @@
         <v>8621.466796875</v>
       </c>
       <c r="O41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13280.4765625</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q41">
+        <v>38</v>
+      </c>
+      <c r="R41">
+        <v>1080.6064453125</v>
+      </c>
+      <c r="S41">
+        <v>14610.392578125</v>
+      </c>
+      <c r="T41">
+        <v>1317.52502441406</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="0"/>
+        <v>13292.867553710939</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5643,7 +7367,7 @@
         <v>7810.0242959973402</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11994.476429402699</v>
       </c>
       <c r="I42">
@@ -5665,11 +7389,27 @@
         <v>9873.07958984375</v>
       </c>
       <c r="O42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14624.51916503907</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <v>39</v>
+      </c>
+      <c r="R42">
+        <v>1136.85546875</v>
+      </c>
+      <c r="S42">
+        <v>15946.0341796875</v>
+      </c>
+      <c r="T42">
+        <v>1306.57495117187</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="0"/>
+        <v>14639.45922851563</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5689,7 +7429,7 @@
         <v>8085.6205429397696</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12275.182850772149</v>
       </c>
       <c r="I43">
@@ -5711,11 +7451,27 @@
         <v>11292.0625</v>
       </c>
       <c r="O43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16142.01684570313</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q43">
+        <v>40</v>
+      </c>
+      <c r="R43">
+        <v>1193.10498046875</v>
+      </c>
+      <c r="S43">
+        <v>17456.83984375</v>
+      </c>
+      <c r="T43">
+        <v>1296.625</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="0"/>
+        <v>16160.21484375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5735,7 +7491,7 @@
         <v>8365.6265165024906</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12560.162711069259</v>
       </c>
       <c r="I44">
@@ -5757,11 +7513,27 @@
         <v>12913.951660156201</v>
       </c>
       <c r="O44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17869.13830566407</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <v>41</v>
+      </c>
+      <c r="R44">
+        <v>1249.3544921875</v>
+      </c>
+      <c r="S44">
+        <v>19179.30859375</v>
+      </c>
+      <c r="T44">
+        <v>1287.72497558593</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="0"/>
+        <v>17891.58361816407</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5781,7 +7553,7 @@
         <v>8650.1856317586498</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12849.56650647421</v>
       </c>
       <c r="I45">
@@ -5803,11 +7575,27 @@
         <v>14787.802734375</v>
       </c>
       <c r="O45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19855.68212890625</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <v>42</v>
+      </c>
+      <c r="R45">
+        <v>1305.603515625</v>
+      </c>
+      <c r="S45">
+        <v>21163.703125</v>
+      </c>
+      <c r="T45">
+        <v>1279.875</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="0"/>
+        <v>19883.828125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5827,7 +7615,7 @@
         <v>8939.4484159048297</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13143.551307365289</v>
       </c>
       <c r="I46">
@@ -5849,11 +7637,27 @@
         <v>16983.987792968699</v>
       </c>
       <c r="O46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22172.77697753907</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q46">
+        <v>43</v>
+      </c>
+      <c r="R46">
+        <v>1361.8525390625</v>
+      </c>
+      <c r="S46">
+        <v>23481.8203125</v>
+      </c>
+      <c r="T46">
+        <v>1273.04992675781</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="0"/>
+        <v>22208.770385742191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5873,7 +7677,7 @@
         <v>9233.5729864415098</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13442.281289642109</v>
       </c>
       <c r="I47">
@@ -5895,11 +7699,27 @@
         <v>19608.48828125</v>
       </c>
       <c r="O47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24926.96008300782</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q47">
+        <v>44</v>
+      </c>
+      <c r="R47">
+        <v>1418.10144042968</v>
+      </c>
+      <c r="S47">
+        <v>26241.376953125</v>
+      </c>
+      <c r="T47">
+        <v>1267.27502441406</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="0"/>
+        <v>24974.101928710941</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5919,7 +7739,7 @@
         <v>9532.7255702292605</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13745.92830052</v>
       </c>
       <c r="I48">
@@ -5941,11 +7761,27 @@
         <v>22831.772949218699</v>
       </c>
       <c r="O48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28288.46398925782</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q48">
+        <v>45</v>
+      </c>
+      <c r="R48">
+        <v>1474.35046386718</v>
+      </c>
+      <c r="S48">
+        <v>29614.365234375</v>
+      </c>
+      <c r="T48">
+        <v>1262.47497558593</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="0"/>
+        <v>28351.89025878907</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -5965,7 +7801,7 @@
         <v>9837.0810676869696</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14054.672463965479</v>
       </c>
       <c r="I49">
@@ -5987,11 +7823,27 @@
         <v>26954.58203125</v>
       </c>
       <c r="O49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32555.649169921879</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q49">
+        <v>46</v>
+      </c>
+      <c r="R49">
+        <v>1530.59948730468</v>
+      </c>
+      <c r="S49">
+        <v>33901.9296875</v>
+      </c>
+      <c r="T49">
+        <v>1258.70007324218</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="0"/>
+        <v>32643.22961425782</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6011,7 +7863,7 @@
         <v>10146.823666926401</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14368.70283132769</v>
       </c>
       <c r="I50">
@@ -6033,11 +7885,27 @@
         <v>32587.23828125</v>
       </c>
       <c r="O50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38331.29150390625</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q50">
+        <v>47</v>
+      </c>
+      <c r="R50">
+        <v>1586.84851074218</v>
+      </c>
+      <c r="S50">
+        <v>39709.84765625</v>
+      </c>
+      <c r="T50">
+        <v>1255.90002441406</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="0"/>
+        <v>38453.947631835938</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6057,7 +7925,7 @@
         <v>10462.147513223301</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14688.21808320379</v>
       </c>
       <c r="I51">
@@ -6079,11 +7947,27 @@
         <v>41309.4482421875</v>
       </c>
       <c r="O51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47177.495361328132</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q51">
+        <v>48</v>
+      </c>
+      <c r="R51">
+        <v>1643.09753417968</v>
+      </c>
+      <c r="S51">
+        <v>48599</v>
+      </c>
+      <c r="T51">
+        <v>1254.07507324218</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="0"/>
+        <v>47344.92492675782</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -6103,7 +7987,7 @@
         <v>10783.257439916701</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15013.427289172319</v>
       </c>
       <c r="I52">
@@ -6125,11 +8009,27 @@
         <v>60474.6513671875</v>
       </c>
       <c r="O52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66418.162475585938</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q52">
+        <v>49</v>
+      </c>
+      <c r="R52">
+        <v>1699.34655761718</v>
+      </c>
+      <c r="S52">
+        <v>67876.1484375</v>
+      </c>
+      <c r="T52">
+        <v>1253.17504882812</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="0"/>
+        <v>66622.973388671875</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -6149,11 +8049,11 @@
         <v>11110.3697676294</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15344.550732746009</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6173,11 +8073,11 @@
         <v>11443.7131796166</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15681.820809744158</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6197,11 +8097,11 @@
         <v>11783.529682115801</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16025.483009291909</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6221,11 +8121,11 @@
         <v>12130.075659799</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16375.796987834581</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6245,11 +8145,11 @@
         <v>12483.623037855599</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16733.037747946291</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6269,11 +8169,11 @@
         <v>12844.4605639035</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17097.496935341271</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6293,11 +8193,11 @@
         <v>13212.8952248655</v>
       </c>
       <c r="G59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17469.484269412653</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6317,11 +8217,11 @@
         <v>13589.2538162324</v>
       </c>
       <c r="G60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17849.32912488006</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6341,11 +8241,11 @@
         <v>13973.884683811</v>
       </c>
       <c r="G61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18237.382284787382</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6365,11 +8265,11 @@
         <v>14367.159661222</v>
       </c>
       <c r="G62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18634.017888234968</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6389,11 +8289,11 @@
         <v>14769.4762301542</v>
       </c>
       <c r="G63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19039.635599963218</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6413,7 +8313,7 @@
         <v>15181.2599348326</v>
       </c>
       <c r="G64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19454.663033338838</v>
       </c>
     </row>
@@ -6437,7 +8337,7 @@
         <v>15602.967087466201</v>
       </c>
       <c r="G65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19879.558463591671</v>
       </c>
     </row>
@@ -6461,7 +8361,7 @@
         <v>16035.087807797699</v>
       </c>
       <c r="G66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20314.813874500349</v>
       </c>
     </row>
@@ -6485,7 +8385,7 @@
         <v>16478.149447522701</v>
       </c>
       <c r="G67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20760.95838935599</v>
       </c>
     </row>
@@ -6509,7 +8409,7 @@
         <v>16932.720459579799</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G107" si="2">C68-D68</f>
+        <f t="shared" ref="G68:G107" si="3">C68-D68</f>
         <v>21218.562146265362</v>
       </c>
     </row>
@@ -6533,7 +8433,7 @@
         <v>17399.414783517601</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21688.240689050559</v>
       </c>
     </row>
@@ -6557,7 +8457,7 @@
         <v>17878.896831809601</v>
       </c>
       <c r="G70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22170.659958659431</v>
       </c>
     </row>
@@ -6581,7 +8481,7 @@
         <v>18371.8871787268</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22666.541986739761</v>
       </c>
     </row>
@@ -6605,7 +8505,7 @@
         <v>18879.1690740087</v>
       </c>
       <c r="G72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23176.67141365225</v>
       </c>
     </row>
@@ -6629,7 +8529,7 @@
         <v>19401.5959291281</v>
       </c>
       <c r="G73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23701.902978751528</v>
       </c>
     </row>
@@ -6653,7 +8553,7 @@
         <v>19940.0999557963</v>
       </c>
       <c r="G74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24243.170162609258</v>
       </c>
     </row>
@@ -6677,7 +8577,7 @@
         <v>20495.7021763015</v>
       </c>
       <c r="G75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24801.49520079928</v>
       </c>
     </row>
@@ -6701,7 +8601,7 @@
         <v>21069.524075703801</v>
       </c>
       <c r="G76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25378.00073929186</v>
       </c>
     </row>
@@ -6725,7 +8625,7 @@
         <v>21662.801230028301</v>
       </c>
       <c r="G77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25973.923465618191</v>
       </c>
     </row>
@@ -6749,7 +8649,7 @@
         <v>22276.899326725499</v>
       </c>
       <c r="G78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26590.630132095321</v>
       </c>
     </row>
@@ -6773,7 +8673,7 @@
         <v>22913.333099715801</v>
       </c>
       <c r="G79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27229.636493443839</v>
       </c>
     </row>
@@ -6797,7 +8697,7 @@
         <v>23573.7888394156</v>
       </c>
       <c r="G80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27892.629819212481</v>
       </c>
     </row>
@@ -6821,7 +8721,7 @@
         <v>24260.151319598001</v>
       </c>
       <c r="G81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28581.495822875841</v>
       </c>
     </row>
@@ -6845,7 +8745,7 @@
         <v>24974.5362237025</v>
       </c>
       <c r="G82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29298.351090233788</v>
       </c>
     </row>
@@ -6869,7 +8769,7 @@
         <v>25719.329476031398</v>
       </c>
       <c r="G83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30045.582412560248</v>
       </c>
     </row>
@@ -6893,7 +8793,7 @@
         <v>26497.235321020999</v>
       </c>
       <c r="G84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30825.894867701041</v>
       </c>
     </row>
@@ -6917,7 +8817,7 @@
         <v>27311.335594631699</v>
       </c>
       <c r="G85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31642.371093174199</v>
       </c>
     </row>
@@ -6941,7 +8841,7 @@
         <v>28165.1634675967</v>
       </c>
       <c r="G86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32498.545031021618</v>
       </c>
     </row>
@@ -6965,7 +8865,7 @@
         <v>29062.7961193788</v>
       </c>
       <c r="G87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33398.494603268722</v>
       </c>
     </row>
@@ -6989,7 +8889,7 @@
         <v>30008.9724916087</v>
       </c>
       <c r="G88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34346.95946677374</v>
       </c>
     </row>
@@ -7013,7 +8913,7 @@
         <v>31009.244733807798</v>
       </c>
       <c r="G89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35349.4924602764</v>
       </c>
     </row>
@@ -7037,7 +8937,7 @@
         <v>32070.175615595399</v>
       </c>
       <c r="G90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36412.65701785063</v>
       </c>
     </row>
@@ -7061,7 +8961,7 @@
         <v>33199.599735502903</v>
       </c>
       <c r="G91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37544.288378890851</v>
       </c>
     </row>
@@ -7085,7 +8985,7 @@
         <v>34406.974986524503</v>
       </c>
       <c r="G92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38753.845054767502</v>
       </c>
     </row>
@@ -7109,7 +9009,7 @@
         <v>35703.864499214702</v>
       </c>
       <c r="G93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40052.890772963103</v>
       </c>
     </row>
@@ -7133,7 +9033,7 @@
         <v>37104.6118835015</v>
       </c>
       <c r="G94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41455.769719867305</v>
       </c>
     </row>
@@ -7157,7 +9057,7 @@
         <v>38627.310980820097</v>
       </c>
       <c r="G95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42980.576293834296</v>
       </c>
     </row>
@@ -7181,7 +9081,7 @@
         <v>40295.239127395798</v>
       </c>
       <c r="G96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44650.588369340716</v>
       </c>
     </row>
@@ -7205,7 +9105,7 @@
         <v>42139.048151407696</v>
       </c>
       <c r="G97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46496.458294973134</v>
       </c>
     </row>
@@ -7229,7 +9129,7 @@
         <v>44200.251275394403</v>
       </c>
       <c r="G98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48559.699796614441</v>
       </c>
     </row>
@@ -7253,7 +9153,7 @@
         <v>46537.050646323602</v>
       </c>
       <c r="G99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50898.515508251432</v>
       </c>
     </row>
@@ -7277,7 +9177,7 @@
         <v>49234.687543300599</v>
       </c>
       <c r="G100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53598.147180381638</v>
       </c>
     </row>
@@ -7301,7 +9201,7 @@
         <v>52425.314787194802</v>
       </c>
       <c r="G101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56790.748090301175</v>
       </c>
     </row>
@@ -7325,7 +9225,7 @@
         <v>56330.326935193501</v>
       </c>
       <c r="G102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60697.713237285592</v>
       </c>
     </row>
@@ -7349,7 +9249,7 @@
         <v>61364.763203099603</v>
       </c>
       <c r="G103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65734.082265481789</v>
       </c>
     </row>
@@ -7373,7 +9273,7 @@
         <v>68460.402594992498</v>
       </c>
       <c r="G104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72831.634594133022</v>
       </c>
     </row>
@@ -7397,7 +9297,7 @@
         <v>80590.478254791597</v>
       </c>
       <c r="G105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84963.603769677313</v>
       </c>
     </row>
@@ -7421,7 +9321,7 @@
         <v>92720.553914590593</v>
       </c>
       <c r="G106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97094.619026924134</v>
       </c>
     </row>
@@ -7445,7 +9345,7 @@
         <v>161180.956509585</v>
       </c>
       <c r="G107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>165555.937857682</v>
       </c>
     </row>
@@ -7456,7 +9356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>